<commit_message>
update docs for publishing
</commit_message>
<xml_diff>
--- a/resources/race-ethnic-data-management/data/race-ethnic-data-management-output-table-ccdph.xlsx
+++ b/resources/race-ethnic-data-management/data/race-ethnic-data-management-output-table-ccdph.xlsx
@@ -1,216 +1,218 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26516"/>
+  <workbookPr/>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_B8923127ADE127FCE687ABC8E71D1B93925953B6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0" refMode="R1C1" iterateCount="0" calcOnSave="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
-  <si>
-    <t xml:space="preserve">Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Source</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Owner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Program</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Question</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Categories</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Secondary Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vital Records: Natality</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IDPH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Epidemiology</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What is the ethnicity of father/co-parent?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hispanic, Mexican, Cuban, Puerto Rican, Other (name of other Hispanic ethnicity)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What is the ethnicity of mother/co-parent?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What is the race of father/co-parent?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">White, Black, Asian, Chinese, Filipino, Vietnamese, Japanese, Korean, Hawaiian, Samoan, Guam, American Indian (name of tribe), Other Asian (name of other Asian race), Other Pacific Islander (name of other Pacific Islander race), Other race (name of other race), Unknown race</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What is the race of mother/co-parent?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ICBRFS/BRFSS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IDPH/CDC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If Asian race, are you...</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asian Indian, Chinese, Filipino, Japanese, Korean, Vietnamese, Other Asian</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If Hispanic, Latino/a, or Spanish origin, are you...</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mecian, Mexican American, Chicago/a, Puerto Rican, Cuban, Another Hispanic, Latino/a, or Spanish origin, Other, Don't know/not sure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If Pacific Islander race, are you?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Native Hawaiian, Guamanian or Chamorro, Samoan, Other Pacific Islander</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What is your ethnicity?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hispanic, Latino/a, or Spanish origin, Not Hispanic, Latino/a, or Spanish origin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Which one of these groups would you say best represents your race?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">White, Black or African American, American Indian or Alaskan Native, Asian, Asian Indian, Chinese, Filipino, Japanese, Korean, Vietnamese, Other Asian, Native Hawaiian, Guamanian or Chamorro, Samoan, Other Pacific Islander, Other race, No preferred race, Multiracial but preferred race not answered, Don’t know/Not sure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Which one or more of the following would you say is your race?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">White, Black or African American, American Indian or Alaskan Native, Asian</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pacific Islander</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Primary Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cook County Health Survey</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CCDPH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hispanic or Latino/a or of Spanish Origin, Not Hispanic or Latino/a or of Spanish Origin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If Hispanic or Latino/a or of Spanish Origin, would you say you are…? (Select Yes or No for each option.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mexican, Mexican-American or Chicgo/a, Puerto Rican, Cuban, Another Hispanic, Latino/a, or Spanish origin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">White, Back or African American, American Indian or Alaska Native, Asian, Native Hawaiian or Pacific Islander, Some other race</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If Asian, would you say you are…? (Select Yes or No for each option.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asian Indian, Chinese, Filipino, Japanese, Korean, Vietnamese, Another Asian origin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vital Records: Mortality</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What is the ethnicity of decedent?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What is the race of decedent?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hospital Discharge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What is the ethnicity of patient?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hispanic or Latino, Non-Hispanic, Declined/Unknown</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What is the race of patient?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">American Indian or Alaska Native, Asian, Black or African American, Native Hawaiian or Other Pacific Islander, White, Two/More, Declined/Unknown, Other</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EMS/Biospatial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">White, Black or African American, American Indian and Alaska Native, Native Hawaiian and Other Pacific Islander, Asian</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I-CARE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Communicable Disease</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hispanic or Latino, Not Hispanic or Latino, Unknown Not Classified</t>
-  </si>
-  <si>
-    <t xml:space="preserve">American Indian or Alaska Native, Asian, Black or African-American, Hispanic or Latino, Middle Eastern or North African, Native Hawaiian or Other Pacific Islander, Other race, Unknown, White</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INEDSS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What is the ethnicity of case?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What is the race of case?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">American Indian or Alaskan Native, Asian, Black or African American, Native Hawaiian or Other Pacific Islander, Unknown, White</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NSSP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hispanic or Latino, Not Categorized, Not Hispanic or Latino, Not Reported or Null, Refused to Answer, Unknown Not Classified</t>
-  </si>
-  <si>
-    <t xml:space="preserve">American Indian or Alaska Native, Asian, Black or African-American, Multiracial, Native Hawaiian or Other Pacific Islander, Not Categorized, Not Reported or Null, Other race, Refused to Answer, White, Unknown</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hispanic or Latino, Not Hispanic or Latino</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What is your race?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">American Indian or Alaska Native, Asian, Black or African American, Native Hawaiian or Other Pacific Islander, White</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="64">
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>Program</t>
+  </si>
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t>Categories</t>
+  </si>
+  <si>
+    <t>Secondary Data</t>
+  </si>
+  <si>
+    <t>Vital Records: Natality</t>
+  </si>
+  <si>
+    <t>IDPH</t>
+  </si>
+  <si>
+    <t>Epidemiology</t>
+  </si>
+  <si>
+    <t>What is the ethnicity of father/co-parent?</t>
+  </si>
+  <si>
+    <t>Hispanic, Mexican, Cuban, Puerto Rican, Other (name of other Hispanic ethnicity)</t>
+  </si>
+  <si>
+    <t>What is the ethnicity of mother/co-parent?</t>
+  </si>
+  <si>
+    <t>What is the race of father/co-parent?</t>
+  </si>
+  <si>
+    <t>White, Black, Asian, Chinese, Filipino, Vietnamese, Japanese, Korean, Hawaiian, Samoan, Guam, American Indian (name of tribe), Other Asian (name of other Asian race), Other Pacific Islander (name of other Pacific Islander race), Other race (name of other race), Unknown race</t>
+  </si>
+  <si>
+    <t>What is the race of mother/co-parent?</t>
+  </si>
+  <si>
+    <t>ICBRFS/BRFSS</t>
+  </si>
+  <si>
+    <t>IDPH/CDC</t>
+  </si>
+  <si>
+    <t>If Asian race, are you...</t>
+  </si>
+  <si>
+    <t>Asian Indian, Chinese, Filipino, Japanese, Korean, Vietnamese, Other Asian</t>
+  </si>
+  <si>
+    <t>If Hispanic, Latino/a, or Spanish origin, are you...</t>
+  </si>
+  <si>
+    <t>Mecian, Mexican American, Chicago/a, Puerto Rican, Cuban, Another Hispanic, Latino/a, or Spanish origin, Other, Don't know/not sure</t>
+  </si>
+  <si>
+    <t>If Pacific Islander race, are you?</t>
+  </si>
+  <si>
+    <t>Native Hawaiian, Guamanian or Chamorro, Samoan, Other Pacific Islander</t>
+  </si>
+  <si>
+    <t>What is your ethnicity?</t>
+  </si>
+  <si>
+    <t>Hispanic, Latino/a, or Spanish origin, Not Hispanic, Latino/a, or Spanish origin</t>
+  </si>
+  <si>
+    <t>Which one of these groups would you say best represents your race?</t>
+  </si>
+  <si>
+    <t>White, Black or African American, American Indian or Alaskan Native, Asian, Asian Indian, Chinese, Filipino, Japanese, Korean, Vietnamese, Other Asian, Native Hawaiian, Guamanian or Chamorro, Samoan, Other Pacific Islander, Other race, No preferred race, Multiracial but preferred race not answered, Don’t know/Not sure</t>
+  </si>
+  <si>
+    <t>Which one or more of the following would you say is your race?</t>
+  </si>
+  <si>
+    <t>White, Black or African American, American Indian or Alaskan Native, Asian</t>
+  </si>
+  <si>
+    <t>Pacific Islander</t>
+  </si>
+  <si>
+    <t>Primary Data</t>
+  </si>
+  <si>
+    <t>Cook County Health Survey</t>
+  </si>
+  <si>
+    <t>CCDPH</t>
+  </si>
+  <si>
+    <t>Hispanic or Latino/a or of Spanish Origin, Not Hispanic or Latino/a or of Spanish Origin</t>
+  </si>
+  <si>
+    <t>If Hispanic or Latino/a or of Spanish Origin, would you say you are…? (Select Yes or No for each option.)</t>
+  </si>
+  <si>
+    <t>Mexican, Mexican-American or Chicgo/a, Puerto Rican, Cuban, Another Hispanic, Latino/a, or Spanish origin</t>
+  </si>
+  <si>
+    <t>White, Back or African American, American Indian or Alaska Native, Asian, Native Hawaiian or Pacific Islander, Some other race</t>
+  </si>
+  <si>
+    <t>If Asian, would you say you are…? (Select Yes or No for each option.)</t>
+  </si>
+  <si>
+    <t>Asian Indian, Chinese, Filipino, Japanese, Korean, Vietnamese, Another Asian origin</t>
+  </si>
+  <si>
+    <t>Vital Records: Mortality</t>
+  </si>
+  <si>
+    <t>What is the ethnicity of decedent?</t>
+  </si>
+  <si>
+    <t>What is the race of decedent?</t>
+  </si>
+  <si>
+    <t>Hospital Discharge</t>
+  </si>
+  <si>
+    <t>What is the ethnicity of patient?</t>
+  </si>
+  <si>
+    <t>Hispanic or Latino, Non-Hispanic, Declined/Unknown</t>
+  </si>
+  <si>
+    <t>What is the race of patient?</t>
+  </si>
+  <si>
+    <t>American Indian or Alaska Native, Asian, Black or African American, Native Hawaiian or Other Pacific Islander, White, Two/More, Declined/Unknown, Other</t>
+  </si>
+  <si>
+    <t>EMS/Biospatial</t>
+  </si>
+  <si>
+    <t>White, Black or African American, American Indian and Alaska Native, Native Hawaiian and Other Pacific Islander, Asian</t>
+  </si>
+  <si>
+    <t>I-CARE</t>
+  </si>
+  <si>
+    <t>Communicable Disease</t>
+  </si>
+  <si>
+    <t>Hispanic or Latino, Not Hispanic or Latino, Unknown Not Classified</t>
+  </si>
+  <si>
+    <t>American Indian or Alaska Native, Asian, Black or African-American, Hispanic or Latino, Middle Eastern or North African, Native Hawaiian or Other Pacific Islander, Other race, Unknown, White</t>
+  </si>
+  <si>
+    <t>INEDSS</t>
+  </si>
+  <si>
+    <t>What is the ethnicity of case?</t>
+  </si>
+  <si>
+    <t>What is the race of case?</t>
+  </si>
+  <si>
+    <t>American Indian or Alaskan Native, Asian, Black or African American, Native Hawaiian or Other Pacific Islander, Unknown, White</t>
+  </si>
+  <si>
+    <t>NSSP</t>
+  </si>
+  <si>
+    <t>Hispanic or Latino, Not Categorized, Not Hispanic or Latino, Not Reported or Null, Refused to Answer, Unknown Not Classified</t>
+  </si>
+  <si>
+    <t>American Indian or Alaska Native, Asian, Black or African-American, Multiracial, Native Hawaiian or Other Pacific Islander, Not Categorized, Not Reported or Null, Other race, Refused to Answer, White, Unknown</t>
+  </si>
+  <si>
+    <t>Hispanic or Latino, Not Hispanic or Latino</t>
+  </si>
+  <si>
+    <t>What is your race?</t>
+  </si>
+  <si>
+    <t>American Indian or Alaska Native, Asian, Black or African American, Native Hawaiian or Other Pacific Islander, White</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -247,6 +249,15 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -528,14 +539,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -555,7 +566,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -575,7 +586,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -595,7 +606,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -615,7 +626,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -635,7 +646,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -655,7 +666,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -675,7 +686,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -695,7 +706,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -715,7 +726,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -735,7 +746,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -755,7 +766,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -775,7 +786,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -795,7 +806,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -815,7 +826,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -835,7 +846,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -855,7 +866,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -875,7 +886,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -895,7 +906,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -915,7 +926,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -935,7 +946,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -955,7 +966,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -975,7 +986,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -995,7 +1006,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -1015,7 +1026,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -1035,7 +1046,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -1055,7 +1066,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>6</v>
       </c>
@@ -1075,7 +1086,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -1095,7 +1106,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -1115,7 +1126,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -1137,6 +1148,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>